<commit_message>
Code divide into the different test cases
</commit_message>
<xml_diff>
--- a/Data/excelData.xlsx
+++ b/Data/excelData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation Projects\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation Projects\RestAPI\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DAA64A0-0182-429A-ABD6-78695DE03216}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FA26F2B-AC9F-4445-B6C1-36D3BA64902D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,10 +33,10 @@
     <t>DealId</t>
   </si>
   <si>
-    <t>337</t>
+    <t>1345860</t>
   </si>
   <si>
-    <t>9612081180088</t>
+    <t>6910214183083</t>
   </si>
 </sst>
 </file>
@@ -365,7 +365,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
6th June Updated c9de and File (Remove SS Debit order with asseration file)
</commit_message>
<xml_diff>
--- a/Data/excelData.xlsx
+++ b/Data/excelData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation Projects\RestAPI\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FA26F2B-AC9F-4445-B6C1-36D3BA64902D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A485B30C-9429-4224-AF9E-ACE3B1F11364}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5115" yWindow="3015" windowWidth="15375" windowHeight="7785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>IdNumber</t>
   </si>
@@ -36,7 +36,13 @@
     <t>1345860</t>
   </si>
   <si>
-    <t>6910214183083</t>
+    <t>337</t>
+  </si>
+  <si>
+    <t>6309108015081</t>
+  </si>
+  <si>
+    <t>0312046845086</t>
   </si>
 </sst>
 </file>
@@ -362,10 +368,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -383,10 +389,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pom and exceldata changes
</commit_message>
<xml_diff>
--- a/Data/excelData.xlsx
+++ b/Data/excelData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation Projects\RestAPI\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ECCF515-3F70-416E-B067-AF56A9FF1B3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6562016E-E0F7-4A34-8D7D-314B06581E53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,21 +39,6 @@
     <t>337</t>
   </si>
   <si>
-    <t>9901290411081</t>
-  </si>
-  <si>
-    <t>6101143713089</t>
-  </si>
-  <si>
-    <t>7208270369087</t>
-  </si>
-  <si>
-    <t>6010217857088</t>
-  </si>
-  <si>
-    <t>5803287313086</t>
-  </si>
-  <si>
     <t>577</t>
   </si>
   <si>
@@ -61,6 +46,21 @@
   </si>
   <si>
     <t>57303</t>
+  </si>
+  <si>
+    <t>8805094764085</t>
+  </si>
+  <si>
+    <t>7601038114086</t>
+  </si>
+  <si>
+    <t>7004045570087</t>
+  </si>
+  <si>
+    <t>9004305546080</t>
+  </si>
+  <si>
+    <t>9507092360085</t>
   </si>
 </sst>
 </file>
@@ -389,7 +389,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -407,7 +407,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>2</v>
@@ -415,7 +415,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>3</v>
@@ -423,26 +423,26 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pom testng and excel data changes
</commit_message>
<xml_diff>
--- a/Data/excelData.xlsx
+++ b/Data/excelData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation Projects\RestAPI\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EB37DB9-F046-4ACB-881A-00FDA01F3417}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13E3245B-6FE7-401B-B2BF-606AC87FF0C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
     <t>533</t>
   </si>
   <si>
-    <t>8908186430084</t>
+    <t>8509031957089</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
pom changes for html report and excel data changes
</commit_message>
<xml_diff>
--- a/Data/excelData.xlsx
+++ b/Data/excelData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation Projects\RestAPI\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C12C7E15-37E8-4CA4-BE67-CA56E43CEB67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC978B31-8E78-40AA-8A65-F7806F5D95B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
     <t>337</t>
   </si>
   <si>
-    <t>9406077747087</t>
+    <t>9203205525083</t>
   </si>
 </sst>
 </file>
@@ -368,7 +368,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
testng file changes for multiple method and new excel data
</commit_message>
<xml_diff>
--- a/Data/excelData.xlsx
+++ b/Data/excelData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation Projects\RestAPI\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35C5BD6C-9CD5-485E-A1DF-EA19C7E1B95C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EFB2A70-22D2-4D29-B3DB-579587CDCF57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
     <t>337</t>
   </si>
   <si>
-    <t>9210193891088</t>
+    <t>9912178036080</t>
   </si>
 </sst>
 </file>
@@ -368,7 +368,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
surifre report comment in pom and new excel data
</commit_message>
<xml_diff>
--- a/Data/excelData.xlsx
+++ b/Data/excelData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation Projects\RestAPI\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF75D2EA-4622-41A4-B7B5-2CEDB6D5B7D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76CFD31E-3E3F-4618-A2A7-965365B643BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
     <t>337</t>
   </si>
   <si>
-    <t>7611153416083</t>
+    <t>0501234885082</t>
   </si>
 </sst>
 </file>
@@ -368,7 +368,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
pom surfier changes again with excel data
</commit_message>
<xml_diff>
--- a/Data/excelData.xlsx
+++ b/Data/excelData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation Projects\RestAPI\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76CFD31E-3E3F-4618-A2A7-965365B643BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1B916DC-169A-46AE-BB7D-F1E6E8D8ECF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
     <t>337</t>
   </si>
   <si>
-    <t>0501234885082</t>
+    <t>7407302046081</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
excel data and get deal file changes.
</commit_message>
<xml_diff>
--- a/Data/excelData.xlsx
+++ b/Data/excelData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation Projects\RestAPI\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73CA6C00-226F-4718-968B-91195A659DE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{687945B3-CCBB-4937-A3FA-68C8F001C104}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
     <t>337</t>
   </si>
   <si>
-    <t>7004232478086</t>
+    <t>0408271821089</t>
   </si>
 </sst>
 </file>
@@ -368,7 +368,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
new excel data for other user
</commit_message>
<xml_diff>
--- a/Data/excelData.xlsx
+++ b/Data/excelData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation Projects\RestAPI\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AAEE382-623D-4186-A839-31256BD7AC31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8421706B-B6C3-418B-8857-2E568D3E4089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5115" yWindow="3015" windowWidth="15375" windowHeight="7785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
     <t>337</t>
   </si>
   <si>
-    <t>9307053027082</t>
+    <t>6912219377082</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
remove selenium dependency and add new excel data.
</commit_message>
<xml_diff>
--- a/Data/excelData.xlsx
+++ b/Data/excelData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation Projects\RestAPI\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8421706B-B6C3-418B-8857-2E568D3E4089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C6E8C8D-562E-4F38-A4D0-92B066F24010}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
     <t>337</t>
   </si>
   <si>
-    <t>6912219377082</t>
+    <t>6708030311080</t>
   </si>
 </sst>
 </file>

</xml_diff>